<commit_message>
modified:   BACKEND/db/db/__pycache__/settings.cpython-312.pyc 	modified:   BACKEND/db/db/settings.py 	modified:   BACKEND/db/db/utils/BRANCHES AND LOCATION.xlsx 	modified:   BACKEND/db/db/utils/import_to_db.py
</commit_message>
<xml_diff>
--- a/BACKEND/db/db/utils/BRANCHES AND LOCATION.xlsx
+++ b/BACKEND/db/db/utils/BRANCHES AND LOCATION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding projects\maps-app\BACKEND\db\db\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{471DFD29-F6DD-4618-B6CB-AB37585B2D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E65BCE-F5CB-4D49-90E1-D7201C77D520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="18735" windowHeight="8385" activeTab="1" xr2:uid="{192655A3-8E6D-440B-BFCA-A5C5173BF4BA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{192655A3-8E6D-440B-BFCA-A5C5173BF4BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1603" uniqueCount="935">
   <si>
     <t>PROVINCE</t>
   </si>
@@ -3140,23 +3140,23 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3529,7 +3529,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3">
@@ -3550,12 +3550,12 @@
       <c r="G2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="28" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="3">
         <v>2</v>
       </c>
@@ -3574,10 +3574,10 @@
       <c r="G3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="27"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="25" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="3">
@@ -3598,12 +3598,12 @@
       <c r="G4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="28" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="7">
         <v>3</v>
       </c>
@@ -3620,10 +3620,10 @@
       <c r="G5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="27"/>
+      <c r="H5" s="29"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="25" t="s">
         <v>62</v>
       </c>
       <c r="B6" s="3">
@@ -3644,12 +3644,12 @@
       <c r="G6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="H6" s="28" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="10" t="s">
         <v>33</v>
       </c>
@@ -3668,10 +3668,10 @@
       <c r="G7" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="26"/>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="3">
         <v>5</v>
       </c>
@@ -3690,10 +3690,10 @@
       <c r="G8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="26"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="3">
         <v>6</v>
       </c>
@@ -3708,10 +3708,10 @@
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="26"/>
+      <c r="H9" s="30"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="7">
         <v>6</v>
       </c>
@@ -3730,10 +3730,10 @@
       <c r="G10" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="H10" s="26"/>
+      <c r="H10" s="30"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="3">
         <v>7</v>
       </c>
@@ -3752,10 +3752,10 @@
       <c r="G11" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H11" s="26"/>
+      <c r="H11" s="30"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="3">
         <v>8</v>
       </c>
@@ -3774,10 +3774,10 @@
       <c r="G12" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="27"/>
+      <c r="H12" s="29"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="25" t="s">
         <v>89</v>
       </c>
       <c r="B13" s="3">
@@ -3798,12 +3798,12 @@
       <c r="G13" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="28" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="3">
         <v>10</v>
       </c>
@@ -3822,10 +3822,10 @@
       <c r="G14" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="26"/>
+      <c r="H14" s="30"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="A15" s="27"/>
       <c r="B15" s="3">
         <v>11</v>
       </c>
@@ -3844,10 +3844,10 @@
       <c r="G15" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="H15" s="26"/>
+      <c r="H15" s="30"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="3">
         <v>12</v>
       </c>
@@ -3866,10 +3866,10 @@
       <c r="G16" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H16" s="26"/>
+      <c r="H16" s="30"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="3">
         <v>13</v>
       </c>
@@ -3888,10 +3888,10 @@
       <c r="G17" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="H17" s="26"/>
+      <c r="H17" s="30"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="3">
         <v>14</v>
       </c>
@@ -3910,10 +3910,10 @@
       <c r="G18" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H18" s="26"/>
+      <c r="H18" s="30"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="3">
         <v>15</v>
       </c>
@@ -3932,10 +3932,10 @@
       <c r="G19" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="H19" s="26"/>
+      <c r="H19" s="30"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="3">
         <v>16</v>
       </c>
@@ -3954,10 +3954,10 @@
       <c r="G20" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H20" s="26"/>
+      <c r="H20" s="30"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="3">
         <v>17</v>
       </c>
@@ -3976,10 +3976,10 @@
       <c r="G21" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="H21" s="26"/>
+      <c r="H21" s="30"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="3">
         <v>18</v>
       </c>
@@ -3998,10 +3998,10 @@
       <c r="G22" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="H22" s="26"/>
+      <c r="H22" s="30"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="3">
         <v>19</v>
       </c>
@@ -4020,10 +4020,10 @@
       <c r="G23" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H23" s="26"/>
+      <c r="H23" s="30"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="3">
         <v>20</v>
       </c>
@@ -4042,10 +4042,10 @@
       <c r="G24" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="H24" s="26"/>
+      <c r="H24" s="30"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="3">
         <v>22</v>
       </c>
@@ -4064,10 +4064,10 @@
       <c r="G25" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="H25" s="27"/>
+      <c r="H25" s="29"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="25" t="s">
         <v>179</v>
       </c>
       <c r="B26" s="10">
@@ -4082,12 +4082,12 @@
       <c r="G26" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H26" s="25" t="s">
+      <c r="H26" s="28" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="3">
         <v>39</v>
       </c>
@@ -4106,10 +4106,10 @@
       <c r="G27" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="H27" s="26"/>
+      <c r="H27" s="30"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="3">
         <v>40</v>
       </c>
@@ -4128,10 +4128,10 @@
       <c r="G28" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="H28" s="26"/>
+      <c r="H28" s="30"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="10" t="s">
         <v>33</v>
       </c>
@@ -4150,10 +4150,10 @@
       <c r="G29" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="H29" s="26"/>
+      <c r="H29" s="30"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="3">
         <v>41</v>
       </c>
@@ -4172,10 +4172,10 @@
       <c r="G30" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="H30" s="26"/>
+      <c r="H30" s="30"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="3">
         <v>42</v>
       </c>
@@ -4194,10 +4194,10 @@
       <c r="G31" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="H31" s="26"/>
+      <c r="H31" s="30"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="3">
         <v>43</v>
       </c>
@@ -4216,7 +4216,7 @@
       <c r="G32" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H32" s="26"/>
+      <c r="H32" s="30"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
@@ -4240,7 +4240,7 @@
       <c r="G33" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="H33" s="27"/>
+      <c r="H33" s="29"/>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="32"/>
@@ -4262,7 +4262,7 @@
       <c r="G34" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="H34" s="25" t="s">
+      <c r="H34" s="28" t="s">
         <v>276</v>
       </c>
     </row>
@@ -4286,7 +4286,7 @@
       <c r="G35" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="H35" s="26"/>
+      <c r="H35" s="30"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="32"/>
@@ -4308,7 +4308,7 @@
       <c r="G36" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="H36" s="26"/>
+      <c r="H36" s="30"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="32"/>
@@ -4330,7 +4330,7 @@
       <c r="G37" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="H37" s="26"/>
+      <c r="H37" s="30"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="32"/>
@@ -4352,7 +4352,7 @@
       <c r="G38" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="H38" s="26"/>
+      <c r="H38" s="30"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="32"/>
@@ -4374,7 +4374,7 @@
       <c r="G39" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="H39" s="26"/>
+      <c r="H39" s="30"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="32"/>
@@ -4396,7 +4396,7 @@
       <c r="G40" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="H40" s="26"/>
+      <c r="H40" s="30"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="32"/>
@@ -4418,7 +4418,7 @@
       <c r="G41" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="H41" s="26"/>
+      <c r="H41" s="30"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="32"/>
@@ -4440,7 +4440,7 @@
       <c r="G42" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="H42" s="26"/>
+      <c r="H42" s="30"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="32"/>
@@ -4462,7 +4462,7 @@
       <c r="G43" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="H43" s="26"/>
+      <c r="H43" s="30"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="32"/>
@@ -4484,7 +4484,7 @@
       <c r="G44" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="H44" s="26"/>
+      <c r="H44" s="30"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="32"/>
@@ -4506,7 +4506,7 @@
       <c r="G45" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="H45" s="26"/>
+      <c r="H45" s="30"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="33"/>
@@ -4528,10 +4528,10 @@
       <c r="G46" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="H46" s="27"/>
+      <c r="H46" s="29"/>
     </row>
     <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="28" t="s">
+      <c r="A47" s="25" t="s">
         <v>225</v>
       </c>
       <c r="B47" s="3">
@@ -4552,12 +4552,12 @@
       <c r="G47" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="H47" s="25" t="s">
+      <c r="H47" s="28" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="29"/>
+      <c r="A48" s="27"/>
       <c r="B48" s="3">
         <v>62</v>
       </c>
@@ -4576,10 +4576,10 @@
       <c r="G48" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="H48" s="26"/>
+      <c r="H48" s="30"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="29"/>
+      <c r="A49" s="27"/>
       <c r="B49" s="3">
         <v>63</v>
       </c>
@@ -4598,10 +4598,10 @@
       <c r="G49" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="H49" s="26"/>
+      <c r="H49" s="30"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="29"/>
+      <c r="A50" s="27"/>
       <c r="B50" s="3">
         <v>64</v>
       </c>
@@ -4620,10 +4620,10 @@
       <c r="G50" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="H50" s="26"/>
+      <c r="H50" s="30"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="29"/>
+      <c r="A51" s="27"/>
       <c r="B51" s="3">
         <v>65</v>
       </c>
@@ -4642,10 +4642,10 @@
       <c r="G51" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="H51" s="26"/>
+      <c r="H51" s="30"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="29"/>
+      <c r="A52" s="27"/>
       <c r="B52" s="3">
         <v>66</v>
       </c>
@@ -4664,10 +4664,10 @@
       <c r="G52" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="H52" s="26"/>
+      <c r="H52" s="30"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="29"/>
+      <c r="A53" s="27"/>
       <c r="B53" s="3">
         <v>67</v>
       </c>
@@ -4686,10 +4686,10 @@
       <c r="G53" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="H53" s="26"/>
+      <c r="H53" s="30"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="29"/>
+      <c r="A54" s="27"/>
       <c r="B54" s="3">
         <v>68</v>
       </c>
@@ -4708,10 +4708,10 @@
       <c r="G54" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="H54" s="26"/>
+      <c r="H54" s="30"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="29"/>
+      <c r="A55" s="27"/>
       <c r="B55" s="3">
         <v>69</v>
       </c>
@@ -4730,10 +4730,10 @@
       <c r="G55" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="H55" s="26"/>
+      <c r="H55" s="30"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="29"/>
+      <c r="A56" s="27"/>
       <c r="B56" s="3">
         <v>76</v>
       </c>
@@ -4752,10 +4752,10 @@
       <c r="G56" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="H56" s="26"/>
+      <c r="H56" s="30"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="30"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="3">
         <v>77</v>
       </c>
@@ -4774,10 +4774,10 @@
       <c r="G57" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="H57" s="27"/>
+      <c r="H57" s="29"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="28" t="s">
+      <c r="A58" s="25" t="s">
         <v>270</v>
       </c>
       <c r="B58" s="3">
@@ -4798,12 +4798,12 @@
       <c r="G58" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="H58" s="25" t="s">
+      <c r="H58" s="28" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="29"/>
+      <c r="A59" s="27"/>
       <c r="B59" s="3">
         <v>71</v>
       </c>
@@ -4822,10 +4822,10 @@
       <c r="G59" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="H59" s="26"/>
+      <c r="H59" s="30"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="29"/>
+      <c r="A60" s="27"/>
       <c r="B60" s="3">
         <v>72</v>
       </c>
@@ -4844,10 +4844,10 @@
       <c r="G60" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="H60" s="26"/>
+      <c r="H60" s="30"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="29"/>
+      <c r="A61" s="27"/>
       <c r="B61" s="17">
         <v>75</v>
       </c>
@@ -4866,10 +4866,10 @@
       <c r="G61" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="H61" s="26"/>
+      <c r="H61" s="30"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
+      <c r="A62" s="26"/>
       <c r="B62" s="3">
         <v>78</v>
       </c>
@@ -4888,17 +4888,10 @@
       <c r="G62" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="H62" s="27"/>
+      <c r="H62" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="A13:A25"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="H13:H25"/>
-    <mergeCell ref="H4:H5"/>
     <mergeCell ref="H26:H33"/>
     <mergeCell ref="H6:H12"/>
     <mergeCell ref="A26:A32"/>
@@ -4908,6 +4901,13 @@
     <mergeCell ref="H47:H57"/>
     <mergeCell ref="H34:H46"/>
     <mergeCell ref="A33:A46"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="A13:A25"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H13:H25"/>
+    <mergeCell ref="H4:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="75" fitToWidth="0" orientation="portrait" r:id="rId1"/>
@@ -4918,8 +4918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{433673A2-E90D-4DAE-8497-A68936D4688C}">
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView tabSelected="1" topLeftCell="C79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H88" sqref="H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7267,6 +7267,9 @@
       </c>
       <c r="F90" s="23" t="s">
         <v>777</v>
+      </c>
+      <c r="G90" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>